<commit_message>
- gestion messageTemplate - interdit update database via cicrequest
</commit_message>
<xml_diff>
--- a/cicaudittrail/Content/uploads/test.xlsx
+++ b/cicaudittrail/Content/uploads/test.xlsx
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>724</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>725</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>726</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>727</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>728</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>729</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>730</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>731</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>732</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>733</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>

</xml_diff>